<commit_message>
added node modules and packages for react client
</commit_message>
<xml_diff>
--- a/mock_up_d3_valuation.xlsx
+++ b/mock_up_d3_valuation.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>WTI</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>express</t>
+  </si>
+  <si>
+    <t>add bootstrap</t>
+  </si>
+  <si>
+    <t>react router</t>
+  </si>
+  <si>
+    <t>React D-3</t>
   </si>
 </sst>
 </file>
@@ -367,8 +376,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449785712"/>
-        <c:axId val="449786104"/>
+        <c:axId val="384242864"/>
+        <c:axId val="384238160"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -448,8 +457,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="451197360"/>
-        <c:axId val="449798256"/>
+        <c:axId val="384243256"/>
+        <c:axId val="384240120"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -598,11 +607,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="449785712"/>
-        <c:axId val="449786104"/>
+        <c:axId val="384242864"/>
+        <c:axId val="384238160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="449785712"/>
+        <c:axId val="384242864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +653,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449786104"/>
+        <c:crossAx val="384238160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -652,7 +661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449786104"/>
+        <c:axId val="384238160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,12 +712,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449785712"/>
+        <c:crossAx val="384242864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="449798256"/>
+        <c:axId val="384240120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,12 +754,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451197360"/>
+        <c:crossAx val="384243256"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="451197360"/>
+        <c:axId val="384243256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +768,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="449798256"/>
+        <c:crossAx val="384240120"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1683,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I23"/>
+  <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,7 +1773,7 @@
         <v>5000</v>
       </c>
       <c r="I4" s="2">
-        <f>H4+I3</f>
+        <f t="shared" ref="I4:I12" si="1">H4+I3</f>
         <v>13000</v>
       </c>
     </row>
@@ -1789,7 +1799,7 @@
         <v>5500</v>
       </c>
       <c r="I5" s="2">
-        <f>H5+I4</f>
+        <f t="shared" si="1"/>
         <v>18500</v>
       </c>
     </row>
@@ -1808,7 +1818,7 @@
         <v>3000</v>
       </c>
       <c r="I6" s="2">
-        <f>H6+I5</f>
+        <f t="shared" si="1"/>
         <v>21500</v>
       </c>
     </row>
@@ -1828,7 +1838,7 @@
         <v>5000</v>
       </c>
       <c r="I7" s="2">
-        <f>H7+I6</f>
+        <f t="shared" si="1"/>
         <v>26500</v>
       </c>
     </row>
@@ -1843,11 +1853,11 @@
         <v>50</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ref="H8:H12" si="1">G8*F8</f>
+        <f t="shared" ref="H8:H11" si="2">G8*F8</f>
         <v>1500</v>
       </c>
       <c r="I8" s="2">
-        <f>H8+I7</f>
+        <f t="shared" si="1"/>
         <v>28000</v>
       </c>
     </row>
@@ -1862,11 +1872,11 @@
         <v>50</v>
       </c>
       <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>1500</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>1500</v>
-      </c>
-      <c r="I9" s="2">
-        <f>H9+I8</f>
         <v>29500</v>
       </c>
     </row>
@@ -1881,11 +1891,11 @@
         <v>100</v>
       </c>
       <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>4000</v>
+      </c>
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
-      <c r="I10" s="2">
-        <f>H10+I9</f>
         <v>33500</v>
       </c>
     </row>
@@ -1900,11 +1910,11 @@
         <v>50</v>
       </c>
       <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>1500</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>1500</v>
-      </c>
-      <c r="I11" s="2">
-        <f>H11+I10</f>
         <v>35000</v>
       </c>
     </row>
@@ -1919,11 +1929,11 @@
         <v>50</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12" si="2">G12*F12</f>
+        <f t="shared" ref="H12" si="3">G12*F12</f>
         <v>1500</v>
       </c>
       <c r="I12" s="2">
-        <f>H12+I11</f>
+        <f t="shared" si="1"/>
         <v>36500</v>
       </c>
     </row>
@@ -2005,6 +2015,30 @@
       </c>
       <c r="B23" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>